<commit_message>
Refactor: make area column optional in excel file uploading. Assume a default area for point type farms.
</commit_message>
<xml_diff>
--- a/monbo-front/public/files/m1-upload-file-template-en.xlsx
+++ b/monbo-front/public/files/m1-upload-file-template-en.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>MANDATORY</t>
   </si>
@@ -543,9 +543,7 @@
       <c r="H1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="I1" s="2"/>
       <c r="J1" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>